<commit_message>
rework for geneology edgelists
marriages edgelist creation started:
csv of uuid for each person in household
started on process to add new member not living in household
</commit_message>
<xml_diff>
--- a/cohesionAndConflict_odkx/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/cohesionAndConflict_odkx/app/config/assets/framework/forms/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2900" yWindow="7580" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="167">
   <si>
     <t>clause</t>
   </si>
@@ -527,6 +527,15 @@
   </si>
   <si>
     <t>Reproductive history</t>
+  </si>
+  <si>
+    <t>marriages</t>
+  </si>
+  <si>
+    <t>Marriages</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('marriages')</t>
   </si>
 </sst>
 </file>
@@ -676,7 +685,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -690,8 +699,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -734,21 +745,22 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1673,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1750,6 +1762,17 @@
       </c>
       <c r="C6" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1766,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.83203125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0"/>
@@ -2090,7 +2113,9 @@
       <c r="H28" s="15"/>
     </row>
     <row r="30" spans="1:8" ht="33" customHeight="1">
-      <c r="A30" s="16"/>
+      <c r="A30" s="16" t="s">
+        <v>164</v>
+      </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -2101,22 +2126,30 @@
     </row>
     <row r="31" spans="1:8" ht="33" customHeight="1">
       <c r="A31" s="18"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="B31" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14" t="s">
+        <v>151</v>
+      </c>
       <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:8" ht="33" customHeight="1">
       <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
       <c r="H32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
families edge creation update
Family table/form creates edgelist between uuids of marriages and child.
</commit_message>
<xml_diff>
--- a/cohesionAndConflict_odkx/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/cohesionAndConflict_odkx/app/config/assets/framework/forms/framework/framework.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="framework_translations" sheetId="3" r:id="rId3"/>
     <sheet name="choices" sheetId="4" r:id="rId4"/>
     <sheet name="survey" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="167">
   <si>
     <t>clause</t>
   </si>
@@ -527,6 +528,15 @@
   </si>
   <si>
     <t>'?' + odkSurvey.getHashString('marriages')</t>
+  </si>
+  <si>
+    <t>families</t>
+  </si>
+  <si>
+    <t>Families</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('families')</t>
   </si>
 </sst>
 </file>
@@ -676,8 +686,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -737,7 +749,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -745,6 +757,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -752,6 +765,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1182,7 +1196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -1676,10 +1690,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1755,6 +1769,17 @@
         <v>162</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1767,10 +1792,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:H28"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.83203125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0"/>
@@ -2122,6 +2147,46 @@
       <c r="G32" s="15"/>
       <c r="H32" s="19"/>
     </row>
+    <row r="34" spans="1:8" ht="33" customHeight="1">
+      <c r="A34" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+    </row>
+    <row r="35" spans="1:8" ht="33" customHeight="1">
+      <c r="A35" s="18"/>
+      <c r="B35" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="H35" s="19"/>
+    </row>
+    <row r="36" spans="1:8" ht="33" customHeight="1">
+      <c r="A36" s="18"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2131,4 +2196,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>